<commit_message>
Empty rows will now be logged and skipped. Added unit tests
</commit_message>
<xml_diff>
--- a/org.matonto.etl.delimited/src/test/resources/testFileWithBlanks.xlsx
+++ b/org.matonto.etl.delimited/src/test/resources/testFileWithBlanks.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Source</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Hexagonal</t>
   </si>
   <si>
-    <t>HfC</t>
-  </si>
-  <si>
     <t>FCC</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
   </si>
   <si>
     <t>ZrN</t>
-  </si>
-  <si>
-    <t>TiB2</t>
-  </si>
-  <si>
-    <t>TiC</t>
   </si>
   <si>
     <t>Cubic</t>
@@ -422,7 +413,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -486,43 +477,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4.6379999999999999</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4.6379999999999999</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4.6379999999999999</v>
-      </c>
-      <c r="G3" s="1">
-        <v>12.76</v>
-      </c>
-      <c r="H3">
-        <v>3900</v>
-      </c>
-      <c r="I3">
-        <v>7052</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>4.5250000000000004</v>
@@ -568,10 +536,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1">
         <v>4.6929999999999996</v>
@@ -597,10 +565,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>4.5780000000000003</v>
@@ -622,69 +590,23 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3.03</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3.12</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3.23</v>
-      </c>
-      <c r="G8" s="1">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="H8">
-        <v>3225</v>
-      </c>
-      <c r="I8">
-        <v>5837</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4.327</v>
-      </c>
-      <c r="E9" s="1">
-        <v>4.327</v>
-      </c>
-      <c r="F9" s="1">
-        <v>4.327</v>
-      </c>
-      <c r="G9" s="1">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="H9">
-        <v>3100</v>
-      </c>
-      <c r="I9">
-        <v>5612</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
         <v>4.242</v>
@@ -708,7 +630,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -737,10 +659,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
         <v>4.4550000000000001</v>
@@ -766,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1">
         <v>4.33</v>
@@ -792,16 +714,16 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1">
         <v>4.6500000000000004</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1">
         <v>3.21</v>

</xml_diff>